<commit_message>
Heat map changes - exclude blank skills
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix v2.xlsx
+++ b/Spreadsheets/Capability Matrix v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="680" windowWidth="28800" windowHeight="16240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16240"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" r:id="rId2"/>
     <sheet name="Survey Sheet" sheetId="5" r:id="rId3"/>
     <sheet name="Input and results" sheetId="1" r:id="rId4"/>
-    <sheet name="Skill Heatmap" sheetId="10" state="hidden" r:id="rId5"/>
-    <sheet name="Planning and Stabilizing Teams" sheetId="9" r:id="rId6"/>
+    <sheet name="Planning and Stabilizing Teams" sheetId="9" r:id="rId5"/>
+    <sheet name="Calculations" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Skills_Header">Settings!#REF!</definedName>
@@ -746,21 +746,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,9 +753,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +770,24 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -12532,28 +12532,28 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:17" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
     </row>
     <row r="2" spans="2:17" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="P2" s="1" t="s">
@@ -12655,7 +12655,7 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="B5:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -12844,14 +12844,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -13324,11 +13324,11 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="15" style="43" customWidth="1"/>
-    <col min="4" max="4" width="17" style="43" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="43" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" style="43" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="15" style="38" customWidth="1"/>
+    <col min="4" max="4" width="17" style="38" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="38" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" style="38" customWidth="1"/>
     <col min="7" max="7" width="31" style="4" customWidth="1"/>
     <col min="8" max="8" width="28.5" customWidth="1"/>
     <col min="9" max="9" width="32.83203125" customWidth="1"/>
@@ -13336,134 +13336,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="55" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:19" s="49" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="50" t="s">
+      <c r="F2" s="47"/>
+      <c r="G2" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-    </row>
-    <row r="3" spans="1:19" s="55" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+    </row>
+    <row r="3" spans="1:19" s="49" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="45" t="s">
         <v>79</v>
       </c>
       <c r="F3"/>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="52" t="str">
+      <c r="H3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B6),"",Settings!$B6)</f>
         <v>Person 1</v>
       </c>
-      <c r="I3" s="52" t="str">
+      <c r="I3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B7),"",Settings!$B7)</f>
         <v>Person 2</v>
       </c>
-      <c r="J3" s="52" t="str">
+      <c r="J3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B8),"",Settings!$B8)</f>
         <v>Team 1</v>
       </c>
-      <c r="K3" s="52" t="str">
+      <c r="K3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B9),"",Settings!$B9)</f>
         <v/>
       </c>
-      <c r="L3" s="52" t="str">
+      <c r="L3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B10),"",Settings!$B10)</f>
         <v/>
       </c>
-      <c r="M3" s="52" t="str">
+      <c r="M3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B11),"",Settings!$B11)</f>
         <v/>
       </c>
-      <c r="N3" s="52" t="str">
+      <c r="N3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B12),"",Settings!$B12)</f>
         <v/>
       </c>
-      <c r="O3" s="52" t="str">
+      <c r="O3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B13),"",Settings!$B13)</f>
         <v/>
       </c>
-      <c r="P3" s="52" t="str">
+      <c r="P3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B14),"",Settings!$B14)</f>
         <v/>
       </c>
-      <c r="Q3" s="52" t="str">
+      <c r="Q3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B15),"",Settings!$B15)</f>
         <v/>
       </c>
-      <c r="R3" s="52" t="str">
+      <c r="R3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B16),"",Settings!$B16)</f>
         <v/>
       </c>
-      <c r="S3" s="52" t="str">
+      <c r="S3" s="46" t="str">
         <f>IF(ISBLANK(Settings!$B17),"",Settings!$B17)</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="str">
+      <c r="A4" s="41" t="str">
         <f>G4</f>
         <v>CSS</v>
       </c>
       <c r="B4" s="19">
-        <f>'Skill Heatmap'!A2</f>
+        <f>Calculations!A2</f>
         <v>0</v>
       </c>
       <c r="C4" s="19">
-        <f>'Skill Heatmap'!B2</f>
+        <f>Calculations!B2</f>
         <v>1</v>
       </c>
       <c r="D4" s="19">
-        <f>'Skill Heatmap'!C2</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="45">
-        <f>'Skill Heatmap'!R2</f>
+        <f>Calculations!C2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="40">
+        <f>Calculations!R2</f>
         <v>2</v>
       </c>
       <c r="F4"/>
-      <c r="G4" s="46" t="str">
+      <c r="G4" s="41" t="str">
         <f>IF(ISBLANK(Settings!D6),"",Settings!D6)</f>
         <v>CSS</v>
       </c>
@@ -13487,28 +13487,28 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="str">
+      <c r="A5" s="41" t="str">
         <f t="shared" ref="A5:A20" si="0">G5</f>
         <v>Javascript</v>
       </c>
       <c r="B5" s="19">
-        <f>'Skill Heatmap'!A3</f>
+        <f>Calculations!A3</f>
         <v>2</v>
       </c>
       <c r="C5" s="19">
-        <f>'Skill Heatmap'!B3</f>
+        <f>Calculations!B3</f>
         <v>0</v>
       </c>
       <c r="D5" s="19">
-        <f>'Skill Heatmap'!C3</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="45">
-        <f>'Skill Heatmap'!R3</f>
+        <f>Calculations!C3</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="40">
+        <f>Calculations!R3</f>
         <v>7</v>
       </c>
       <c r="F5"/>
-      <c r="G5" s="46" t="str">
+      <c r="G5" s="41" t="str">
         <f>IF(ISBLANK(Settings!D7),"",Settings!D7)</f>
         <v>Javascript</v>
       </c>
@@ -13532,28 +13532,28 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="str">
+      <c r="A6" s="41" t="str">
         <f t="shared" si="0"/>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B6" s="19">
-        <f>'Skill Heatmap'!A4</f>
+        <f>Calculations!A4</f>
         <v>1</v>
       </c>
       <c r="C6" s="19">
-        <f>'Skill Heatmap'!B4</f>
+        <f>Calculations!B4</f>
         <v>1</v>
       </c>
       <c r="D6" s="19">
-        <f>'Skill Heatmap'!C4</f>
+        <f>Calculations!C4</f>
         <v>1</v>
       </c>
-      <c r="E6" s="45">
-        <f>'Skill Heatmap'!R4</f>
+      <c r="E6" s="40">
+        <f>Calculations!R4</f>
         <v>6</v>
       </c>
       <c r="F6"/>
-      <c r="G6" s="46" t="str">
+      <c r="G6" s="41" t="str">
         <f>IF(ISBLANK(Settings!D8),"",Settings!D8)</f>
         <v>DB Backup/Restore</v>
       </c>
@@ -13577,28 +13577,28 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="str">
+      <c r="A7" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B7" s="19" t="str">
-        <f>'Skill Heatmap'!A5</f>
+        <f>Calculations!A5</f>
         <v/>
       </c>
       <c r="C7" s="19" t="str">
-        <f>'Skill Heatmap'!B5</f>
+        <f>Calculations!B5</f>
         <v/>
       </c>
       <c r="D7" s="19" t="str">
-        <f>'Skill Heatmap'!C5</f>
-        <v/>
-      </c>
-      <c r="E7" s="45">
-        <f>'Skill Heatmap'!R5</f>
-        <v>0</v>
+        <f>Calculations!C5</f>
+        <v/>
+      </c>
+      <c r="E7" s="40" t="str">
+        <f>Calculations!R5</f>
+        <v/>
       </c>
       <c r="F7"/>
-      <c r="G7" s="46" t="str">
+      <c r="G7" s="41" t="str">
         <f>IF(ISBLANK(Settings!D9),"",Settings!D9)</f>
         <v/>
       </c>
@@ -13616,28 +13616,28 @@
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="str">
+      <c r="A8" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B8" s="19" t="str">
-        <f>'Skill Heatmap'!A6</f>
+        <f>Calculations!A6</f>
         <v/>
       </c>
       <c r="C8" s="19" t="str">
-        <f>'Skill Heatmap'!B6</f>
+        <f>Calculations!B6</f>
         <v/>
       </c>
       <c r="D8" s="19" t="str">
-        <f>'Skill Heatmap'!C6</f>
-        <v/>
-      </c>
-      <c r="E8" s="45">
-        <f>'Skill Heatmap'!R6</f>
-        <v>0</v>
+        <f>Calculations!C6</f>
+        <v/>
+      </c>
+      <c r="E8" s="40" t="str">
+        <f>Calculations!R6</f>
+        <v/>
       </c>
       <c r="F8"/>
-      <c r="G8" s="46" t="str">
+      <c r="G8" s="41" t="str">
         <f>IF(ISBLANK(Settings!D10),"",Settings!D10)</f>
         <v/>
       </c>
@@ -13655,28 +13655,28 @@
       <c r="S8" s="16"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="str">
+      <c r="A9" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B9" s="19" t="str">
-        <f>'Skill Heatmap'!A7</f>
+        <f>Calculations!A7</f>
         <v/>
       </c>
       <c r="C9" s="19" t="str">
-        <f>'Skill Heatmap'!B7</f>
+        <f>Calculations!B7</f>
         <v/>
       </c>
       <c r="D9" s="19" t="str">
-        <f>'Skill Heatmap'!C7</f>
-        <v/>
-      </c>
-      <c r="E9" s="45">
-        <f>'Skill Heatmap'!R7</f>
-        <v>0</v>
+        <f>Calculations!C7</f>
+        <v/>
+      </c>
+      <c r="E9" s="40" t="str">
+        <f>Calculations!R7</f>
+        <v/>
       </c>
       <c r="F9"/>
-      <c r="G9" s="46" t="str">
+      <c r="G9" s="41" t="str">
         <f>IF(ISBLANK(Settings!D11),"",Settings!D11)</f>
         <v/>
       </c>
@@ -13694,28 +13694,28 @@
       <c r="S9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="str">
+      <c r="A10" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B10" s="19" t="str">
-        <f>'Skill Heatmap'!A8</f>
+        <f>Calculations!A8</f>
         <v/>
       </c>
       <c r="C10" s="19" t="str">
-        <f>'Skill Heatmap'!B8</f>
+        <f>Calculations!B8</f>
         <v/>
       </c>
       <c r="D10" s="19" t="str">
-        <f>'Skill Heatmap'!C8</f>
-        <v/>
-      </c>
-      <c r="E10" s="45">
-        <f>'Skill Heatmap'!R8</f>
-        <v>0</v>
+        <f>Calculations!C8</f>
+        <v/>
+      </c>
+      <c r="E10" s="40" t="str">
+        <f>Calculations!R8</f>
+        <v/>
       </c>
       <c r="F10"/>
-      <c r="G10" s="46" t="str">
+      <c r="G10" s="41" t="str">
         <f>IF(ISBLANK(Settings!D12),"",Settings!D12)</f>
         <v/>
       </c>
@@ -13733,28 +13733,28 @@
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="str">
+      <c r="A11" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B11" s="19" t="str">
-        <f>'Skill Heatmap'!A9</f>
+        <f>Calculations!A9</f>
         <v/>
       </c>
       <c r="C11" s="19" t="str">
-        <f>'Skill Heatmap'!B9</f>
+        <f>Calculations!B9</f>
         <v/>
       </c>
       <c r="D11" s="19" t="str">
-        <f>'Skill Heatmap'!C9</f>
-        <v/>
-      </c>
-      <c r="E11" s="45">
-        <f>'Skill Heatmap'!R9</f>
-        <v>0</v>
+        <f>Calculations!C9</f>
+        <v/>
+      </c>
+      <c r="E11" s="40" t="str">
+        <f>Calculations!R9</f>
+        <v/>
       </c>
       <c r="F11"/>
-      <c r="G11" s="46" t="str">
+      <c r="G11" s="41" t="str">
         <f>IF(ISBLANK(Settings!D13),"",Settings!D13)</f>
         <v/>
       </c>
@@ -13772,28 +13772,28 @@
       <c r="S11" s="16"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="str">
+      <c r="A12" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B12" s="19" t="str">
-        <f>'Skill Heatmap'!A10</f>
+        <f>Calculations!A10</f>
         <v/>
       </c>
       <c r="C12" s="19" t="str">
-        <f>'Skill Heatmap'!B10</f>
+        <f>Calculations!B10</f>
         <v/>
       </c>
       <c r="D12" s="19" t="str">
-        <f>'Skill Heatmap'!C10</f>
-        <v/>
-      </c>
-      <c r="E12" s="45">
-        <f>'Skill Heatmap'!R10</f>
-        <v>0</v>
+        <f>Calculations!C10</f>
+        <v/>
+      </c>
+      <c r="E12" s="40" t="str">
+        <f>Calculations!R10</f>
+        <v/>
       </c>
       <c r="F12"/>
-      <c r="G12" s="46" t="str">
+      <c r="G12" s="41" t="str">
         <f>IF(ISBLANK(Settings!D14),"",Settings!D14)</f>
         <v/>
       </c>
@@ -13811,28 +13811,28 @@
       <c r="S12" s="16"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="str">
+      <c r="A13" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B13" s="19" t="str">
-        <f>'Skill Heatmap'!A11</f>
+        <f>Calculations!A11</f>
         <v/>
       </c>
       <c r="C13" s="19" t="str">
-        <f>'Skill Heatmap'!B11</f>
+        <f>Calculations!B11</f>
         <v/>
       </c>
       <c r="D13" s="19" t="str">
-        <f>'Skill Heatmap'!C11</f>
-        <v/>
-      </c>
-      <c r="E13" s="45">
-        <f>'Skill Heatmap'!R11</f>
-        <v>0</v>
+        <f>Calculations!C11</f>
+        <v/>
+      </c>
+      <c r="E13" s="40" t="str">
+        <f>Calculations!R11</f>
+        <v/>
       </c>
       <c r="F13"/>
-      <c r="G13" s="46" t="str">
+      <c r="G13" s="41" t="str">
         <f>IF(ISBLANK(Settings!D15),"",Settings!D15)</f>
         <v/>
       </c>
@@ -13850,28 +13850,28 @@
       <c r="S13" s="16"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="str">
+      <c r="A14" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B14" s="19" t="str">
-        <f>'Skill Heatmap'!A12</f>
+        <f>Calculations!A12</f>
         <v/>
       </c>
       <c r="C14" s="19" t="str">
-        <f>'Skill Heatmap'!B12</f>
+        <f>Calculations!B12</f>
         <v/>
       </c>
       <c r="D14" s="19" t="str">
-        <f>'Skill Heatmap'!C12</f>
-        <v/>
-      </c>
-      <c r="E14" s="45">
-        <f>'Skill Heatmap'!R12</f>
-        <v>0</v>
+        <f>Calculations!C12</f>
+        <v/>
+      </c>
+      <c r="E14" s="40" t="str">
+        <f>Calculations!R12</f>
+        <v/>
       </c>
       <c r="F14"/>
-      <c r="G14" s="46" t="str">
+      <c r="G14" s="41" t="str">
         <f>IF(ISBLANK(Settings!D16),"",Settings!D16)</f>
         <v/>
       </c>
@@ -13889,28 +13889,28 @@
       <c r="S14" s="16"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="str">
+      <c r="A15" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B15" s="19" t="str">
-        <f>'Skill Heatmap'!A13</f>
+        <f>Calculations!A13</f>
         <v/>
       </c>
       <c r="C15" s="19" t="str">
-        <f>'Skill Heatmap'!B13</f>
+        <f>Calculations!B13</f>
         <v/>
       </c>
       <c r="D15" s="19" t="str">
-        <f>'Skill Heatmap'!C13</f>
-        <v/>
-      </c>
-      <c r="E15" s="45">
-        <f>'Skill Heatmap'!R13</f>
-        <v>0</v>
+        <f>Calculations!C13</f>
+        <v/>
+      </c>
+      <c r="E15" s="40" t="str">
+        <f>Calculations!R13</f>
+        <v/>
       </c>
       <c r="F15"/>
-      <c r="G15" s="46" t="str">
+      <c r="G15" s="41" t="str">
         <f>IF(ISBLANK(Settings!D17),"",Settings!D17)</f>
         <v/>
       </c>
@@ -13928,28 +13928,28 @@
       <c r="S15" s="16"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="str">
+      <c r="A16" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B16" s="19" t="str">
-        <f>'Skill Heatmap'!A14</f>
+        <f>Calculations!A14</f>
         <v/>
       </c>
       <c r="C16" s="19" t="str">
-        <f>'Skill Heatmap'!B14</f>
+        <f>Calculations!B14</f>
         <v/>
       </c>
       <c r="D16" s="19" t="str">
-        <f>'Skill Heatmap'!C14</f>
-        <v/>
-      </c>
-      <c r="E16" s="45">
-        <f>'Skill Heatmap'!R14</f>
-        <v>0</v>
+        <f>Calculations!C14</f>
+        <v/>
+      </c>
+      <c r="E16" s="40" t="str">
+        <f>Calculations!R14</f>
+        <v/>
       </c>
       <c r="F16"/>
-      <c r="G16" s="46" t="str">
+      <c r="G16" s="41" t="str">
         <f>IF(ISBLANK(Settings!D18),"",Settings!D18)</f>
         <v/>
       </c>
@@ -13967,28 +13967,28 @@
       <c r="S16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="str">
+      <c r="A17" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B17" s="19" t="str">
-        <f>'Skill Heatmap'!A15</f>
+        <f>Calculations!A15</f>
         <v/>
       </c>
       <c r="C17" s="19" t="str">
-        <f>'Skill Heatmap'!B15</f>
+        <f>Calculations!B15</f>
         <v/>
       </c>
       <c r="D17" s="19" t="str">
-        <f>'Skill Heatmap'!C15</f>
-        <v/>
-      </c>
-      <c r="E17" s="45">
-        <f>'Skill Heatmap'!R15</f>
-        <v>0</v>
+        <f>Calculations!C15</f>
+        <v/>
+      </c>
+      <c r="E17" s="40" t="str">
+        <f>Calculations!R15</f>
+        <v/>
       </c>
       <c r="F17"/>
-      <c r="G17" s="46" t="str">
+      <c r="G17" s="41" t="str">
         <f>IF(ISBLANK(Settings!D19),"",Settings!D19)</f>
         <v/>
       </c>
@@ -14006,28 +14006,28 @@
       <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="str">
+      <c r="A18" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B18" s="19" t="str">
-        <f>'Skill Heatmap'!A16</f>
+        <f>Calculations!A16</f>
         <v/>
       </c>
       <c r="C18" s="19" t="str">
-        <f>'Skill Heatmap'!B16</f>
+        <f>Calculations!B16</f>
         <v/>
       </c>
       <c r="D18" s="19" t="str">
-        <f>'Skill Heatmap'!C16</f>
-        <v/>
-      </c>
-      <c r="E18" s="45">
-        <f>'Skill Heatmap'!R16</f>
-        <v>0</v>
+        <f>Calculations!C16</f>
+        <v/>
+      </c>
+      <c r="E18" s="40" t="str">
+        <f>Calculations!R16</f>
+        <v/>
       </c>
       <c r="F18"/>
-      <c r="G18" s="46" t="str">
+      <c r="G18" s="41" t="str">
         <f>IF(ISBLANK(Settings!D20),"",Settings!D20)</f>
         <v/>
       </c>
@@ -14045,28 +14045,28 @@
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="str">
+      <c r="A19" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B19" s="19" t="str">
-        <f>'Skill Heatmap'!A17</f>
+        <f>Calculations!A17</f>
         <v/>
       </c>
       <c r="C19" s="19" t="str">
-        <f>'Skill Heatmap'!B17</f>
+        <f>Calculations!B17</f>
         <v/>
       </c>
       <c r="D19" s="19" t="str">
-        <f>'Skill Heatmap'!C17</f>
-        <v/>
-      </c>
-      <c r="E19" s="45">
-        <f>'Skill Heatmap'!R17</f>
-        <v>0</v>
+        <f>Calculations!C17</f>
+        <v/>
+      </c>
+      <c r="E19" s="40" t="str">
+        <f>Calculations!R17</f>
+        <v/>
       </c>
       <c r="F19"/>
-      <c r="G19" s="46" t="str">
+      <c r="G19" s="41" t="str">
         <f>IF(ISBLANK(Settings!D21),"",Settings!D21)</f>
         <v/>
       </c>
@@ -14084,28 +14084,28 @@
       <c r="S19" s="16"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="str">
+      <c r="A20" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B20" s="19" t="str">
-        <f>'Skill Heatmap'!A18</f>
+        <f>Calculations!A18</f>
         <v/>
       </c>
       <c r="C20" s="19" t="str">
-        <f>'Skill Heatmap'!B18</f>
+        <f>Calculations!B18</f>
         <v/>
       </c>
       <c r="D20" s="19" t="str">
-        <f>'Skill Heatmap'!C18</f>
-        <v/>
-      </c>
-      <c r="E20" s="45">
-        <f>'Skill Heatmap'!R18</f>
-        <v>0</v>
+        <f>Calculations!C18</f>
+        <v/>
+      </c>
+      <c r="E20" s="40" t="str">
+        <f>Calculations!R18</f>
+        <v/>
       </c>
       <c r="F20"/>
-      <c r="G20" s="46" t="str">
+      <c r="G20" s="41" t="str">
         <f>IF(ISBLANK(Settings!D22),"",Settings!D22)</f>
         <v/>
       </c>
@@ -14170,11 +14170,11 @@
       <c r="G30"/>
     </row>
     <row r="31" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14262,17 +14262,456 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N58"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="56"/>
+      <c r="I5" s="57"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="22">
+        <v>0</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>1</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>9</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="21">
+        <v>0</v>
+      </c>
+      <c r="C40" s="21">
+        <v>1</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="21">
+        <v>0</v>
+      </c>
+      <c r="B41" s="28">
+        <v>9</v>
+      </c>
+      <c r="C41" s="29">
+        <v>7</v>
+      </c>
+      <c r="D41" s="30">
+        <v>3</v>
+      </c>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="21">
+        <v>1</v>
+      </c>
+      <c r="B42" s="31">
+        <v>8</v>
+      </c>
+      <c r="C42" s="32">
+        <v>5</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="34">
+        <v>6</v>
+      </c>
+      <c r="C43" s="35">
+        <v>4</v>
+      </c>
+      <c r="D43" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:I5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B7:D9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:I9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="43" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="38" customWidth="1"/>
     <col min="4" max="4" width="4.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="18" width="13" customWidth="1"/>
@@ -14342,16 +14781,16 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="43">
-        <f>IF($E2&lt;&gt;"",COUNTIF($F2:$Q2, "&gt;= 3"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="43">
-        <f>IF($E2&lt;&gt;"",COUNTIF($F2:$Q2, "= 2"),"")</f>
+      <c r="A2" s="38">
+        <f t="shared" ref="A2:A18" si="0">IF($E2&lt;&gt;"",COUNTIF($F2:$Q2, "&gt;= 3"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="38">
+        <f t="shared" ref="B2:B18" si="1">IF($E2&lt;&gt;"",COUNTIF($F2:$Q2, "= 2"),"")</f>
         <v>1</v>
       </c>
-      <c r="C2" s="43">
-        <f>IF($E2&lt;&gt;"",COUNTIF($F2:$Q2, "= 1"),"")</f>
+      <c r="C2" s="38">
+        <f t="shared" ref="C2:C18" si="2">IF($E2&lt;&gt;"",COUNTIF($F2:$Q2, "= 1"),"")</f>
         <v>0</v>
       </c>
       <c r="E2" s="1" t="str">
@@ -14406,22 +14845,22 @@
         <f>IFERROR(MATCH('Input and results'!S4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R2" s="44">
-        <f>SUM(F2:Q2)</f>
+      <c r="R2" s="39">
+        <f>IF(SUM(F2:Q2)&gt;0,SUM(F2:Q2),"")</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="43">
-        <f>IF($E3&lt;&gt;"",COUNTIF($F3:$Q3, "&gt;= 3"),"")</f>
+      <c r="A3" s="38">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="43">
-        <f>IF($E3&lt;&gt;"",COUNTIF($F3:$Q3, "= 2"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="43">
-        <f>IF($E3&lt;&gt;"",COUNTIF($F3:$Q3, "= 1"),"")</f>
+      <c r="B3" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="38">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E3" s="1" t="str">
@@ -14476,22 +14915,22 @@
         <f>IFERROR(MATCH('Input and results'!S5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="44">
-        <f>SUM(F3:Q3)</f>
+      <c r="R3" s="39">
+        <f t="shared" ref="R3:R18" si="3">IF(SUM(F3:Q3)&gt;0,SUM(F3:Q3),"")</f>
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="43">
-        <f>IF($E4&lt;&gt;"",COUNTIF($F4:$Q4, "&gt;= 3"),"")</f>
+      <c r="A4" s="38">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B4" s="43">
-        <f>IF($E4&lt;&gt;"",COUNTIF($F4:$Q4, "= 2"),"")</f>
+      <c r="B4" s="38">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C4" s="43">
-        <f>IF($E4&lt;&gt;"",COUNTIF($F4:$Q4, "= 1"),"")</f>
+      <c r="C4" s="38">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E4" s="1" t="str">
@@ -14546,22 +14985,22 @@
         <f>IFERROR(MATCH('Input and results'!S6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="44">
-        <f>SUM(F4:Q4)</f>
+      <c r="R4" s="39">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="str">
-        <f>IF($E5&lt;&gt;"",COUNTIF($F5:$Q5, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B5" s="43" t="str">
-        <f>IF($E5&lt;&gt;"",COUNTIF($F5:$Q5, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C5" s="43" t="str">
-        <f>IF($E5&lt;&gt;"",COUNTIF($F5:$Q5, "= 1"),"")</f>
+      <c r="A5" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B5" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C5" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E5" s="1" t="str">
@@ -14616,22 +15055,22 @@
         <f>IFERROR(MATCH('Input and results'!S7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="44">
-        <f>SUM(F5:Q5)</f>
-        <v>0</v>
+      <c r="R5" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="str">
-        <f>IF($E6&lt;&gt;"",COUNTIF($F6:$Q6, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B6" s="43" t="str">
-        <f>IF($E6&lt;&gt;"",COUNTIF($F6:$Q6, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C6" s="43" t="str">
-        <f>IF($E6&lt;&gt;"",COUNTIF($F6:$Q6, "= 1"),"")</f>
+      <c r="A6" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B6" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C6" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E6" s="1" t="str">
@@ -14686,22 +15125,22 @@
         <f>IFERROR(MATCH('Input and results'!S8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="44">
-        <f>SUM(F6:Q6)</f>
-        <v>0</v>
+      <c r="R6" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="str">
-        <f>IF($E7&lt;&gt;"",COUNTIF($F7:$Q7, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B7" s="43" t="str">
-        <f>IF($E7&lt;&gt;"",COUNTIF($F7:$Q7, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C7" s="43" t="str">
-        <f>IF($E7&lt;&gt;"",COUNTIF($F7:$Q7, "= 1"),"")</f>
+      <c r="A7" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B7" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C7" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E7" s="1" t="str">
@@ -14756,22 +15195,22 @@
         <f>IFERROR(MATCH('Input and results'!S9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="44">
-        <f>SUM(F7:Q7)</f>
-        <v>0</v>
+      <c r="R7" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="str">
-        <f>IF($E8&lt;&gt;"",COUNTIF($F8:$Q8, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B8" s="43" t="str">
-        <f>IF($E8&lt;&gt;"",COUNTIF($F8:$Q8, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C8" s="43" t="str">
-        <f>IF($E8&lt;&gt;"",COUNTIF($F8:$Q8, "= 1"),"")</f>
+      <c r="A8" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B8" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C8" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E8" s="1" t="str">
@@ -14826,22 +15265,22 @@
         <f>IFERROR(MATCH('Input and results'!S10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="44">
-        <f>SUM(F8:Q8)</f>
-        <v>0</v>
+      <c r="R8" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="str">
-        <f>IF($E9&lt;&gt;"",COUNTIF($F9:$Q9, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B9" s="43" t="str">
-        <f>IF($E9&lt;&gt;"",COUNTIF($F9:$Q9, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="43" t="str">
-        <f>IF($E9&lt;&gt;"",COUNTIF($F9:$Q9, "= 1"),"")</f>
+      <c r="A9" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B9" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C9" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E9" s="1" t="str">
@@ -14896,22 +15335,22 @@
         <f>IFERROR(MATCH('Input and results'!S11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="44">
-        <f>SUM(F9:Q9)</f>
-        <v>0</v>
+      <c r="R9" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="str">
-        <f>IF($E10&lt;&gt;"",COUNTIF($F10:$Q10, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B10" s="43" t="str">
-        <f>IF($E10&lt;&gt;"",COUNTIF($F10:$Q10, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C10" s="43" t="str">
-        <f>IF($E10&lt;&gt;"",COUNTIF($F10:$Q10, "= 1"),"")</f>
+      <c r="A10" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B10" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C10" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E10" s="1" t="str">
@@ -14966,22 +15405,22 @@
         <f>IFERROR(MATCH('Input and results'!S12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="44">
-        <f>SUM(F10:Q10)</f>
-        <v>0</v>
+      <c r="R10" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="str">
-        <f>IF($E11&lt;&gt;"",COUNTIF($F11:$Q11, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B11" s="43" t="str">
-        <f>IF($E11&lt;&gt;"",COUNTIF($F11:$Q11, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C11" s="43" t="str">
-        <f>IF($E11&lt;&gt;"",COUNTIF($F11:$Q11, "= 1"),"")</f>
+      <c r="A11" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B11" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E11" s="1" t="str">
@@ -15036,22 +15475,22 @@
         <f>IFERROR(MATCH('Input and results'!S13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R11" s="44">
-        <f>SUM(F11:Q11)</f>
-        <v>0</v>
+      <c r="R11" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="str">
-        <f>IF($E12&lt;&gt;"",COUNTIF($F12:$Q12, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B12" s="43" t="str">
-        <f>IF($E12&lt;&gt;"",COUNTIF($F12:$Q12, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="43" t="str">
-        <f>IF($E12&lt;&gt;"",COUNTIF($F12:$Q12, "= 1"),"")</f>
+      <c r="A12" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B12" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C12" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E12" s="1" t="str">
@@ -15106,22 +15545,22 @@
         <f>IFERROR(MATCH('Input and results'!S14,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="44">
-        <f>SUM(F12:Q12)</f>
-        <v>0</v>
+      <c r="R12" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="str">
-        <f>IF($E13&lt;&gt;"",COUNTIF($F13:$Q13, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B13" s="43" t="str">
-        <f>IF($E13&lt;&gt;"",COUNTIF($F13:$Q13, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C13" s="43" t="str">
-        <f>IF($E13&lt;&gt;"",COUNTIF($F13:$Q13, "= 1"),"")</f>
+      <c r="A13" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B13" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C13" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E13" s="1" t="str">
@@ -15176,22 +15615,22 @@
         <f>IFERROR(MATCH('Input and results'!S15,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="44">
-        <f>SUM(F13:Q13)</f>
-        <v>0</v>
+      <c r="R13" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="str">
-        <f>IF($E14&lt;&gt;"",COUNTIF($F14:$Q14, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B14" s="43" t="str">
-        <f>IF($E14&lt;&gt;"",COUNTIF($F14:$Q14, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="43" t="str">
-        <f>IF($E14&lt;&gt;"",COUNTIF($F14:$Q14, "= 1"),"")</f>
+      <c r="A14" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B14" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C14" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E14" s="1" t="str">
@@ -15246,22 +15685,22 @@
         <f>IFERROR(MATCH('Input and results'!S16,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="44">
-        <f>SUM(F14:Q14)</f>
-        <v>0</v>
+      <c r="R14" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="str">
-        <f>IF($E15&lt;&gt;"",COUNTIF($F15:$Q15, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B15" s="43" t="str">
-        <f>IF($E15&lt;&gt;"",COUNTIF($F15:$Q15, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="43" t="str">
-        <f>IF($E15&lt;&gt;"",COUNTIF($F15:$Q15, "= 1"),"")</f>
+      <c r="A15" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B15" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C15" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E15" s="1" t="str">
@@ -15316,22 +15755,22 @@
         <f>IFERROR(MATCH('Input and results'!S17,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R15" s="44">
-        <f>SUM(F15:Q15)</f>
-        <v>0</v>
+      <c r="R15" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="str">
-        <f>IF($E16&lt;&gt;"",COUNTIF($F16:$Q16, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B16" s="43" t="str">
-        <f>IF($E16&lt;&gt;"",COUNTIF($F16:$Q16, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="43" t="str">
-        <f>IF($E16&lt;&gt;"",COUNTIF($F16:$Q16, "= 1"),"")</f>
+      <c r="A16" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B16" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C16" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E16" s="1" t="str">
@@ -15386,22 +15825,22 @@
         <f>IFERROR(MATCH('Input and results'!S18,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R16" s="44">
-        <f>SUM(F16:Q16)</f>
-        <v>0</v>
+      <c r="R16" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="str">
-        <f>IF($E17&lt;&gt;"",COUNTIF($F17:$Q17, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="43" t="str">
-        <f>IF($E17&lt;&gt;"",COUNTIF($F17:$Q17, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="43" t="str">
-        <f>IF($E17&lt;&gt;"",COUNTIF($F17:$Q17, "= 1"),"")</f>
+      <c r="A17" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B17" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C17" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E17" s="1" t="str">
@@ -15456,22 +15895,22 @@
         <f>IFERROR(MATCH('Input and results'!S19,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R17" s="44">
-        <f>SUM(F17:Q17)</f>
-        <v>0</v>
+      <c r="R17" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="str">
-        <f>IF($E18&lt;&gt;"",COUNTIF($F18:$Q18, "&gt;= 3"),"")</f>
-        <v/>
-      </c>
-      <c r="B18" s="43" t="str">
-        <f>IF($E18&lt;&gt;"",COUNTIF($F18:$Q18, "= 2"),"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="43" t="str">
-        <f>IF($E18&lt;&gt;"",COUNTIF($F18:$Q18, "= 1"),"")</f>
+      <c r="A18" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B18" s="38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="38" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E18" s="1" t="str">
@@ -15526,9 +15965,9 @@
         <f>IFERROR(MATCH('Input and results'!S20,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="44">
-        <f>SUM(F18:Q18)</f>
-        <v>0</v>
+      <c r="R18" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -15616,443 +16055,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N58"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="22">
-        <v>0</v>
-      </c>
-      <c r="C6" s="22">
-        <v>1</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="21">
-        <v>0</v>
-      </c>
-      <c r="H6" s="21">
-        <v>1</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="F7" s="21">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>9</v>
-      </c>
-      <c r="H7" s="3">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2</v>
-      </c>
-      <c r="F8" s="21">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8</v>
-      </c>
-      <c r="H8" s="3">
-        <v>5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="3">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="3">
-        <v>6</v>
-      </c>
-      <c r="H9" s="3">
-        <v>4</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="24"/>
-    </row>
-    <row r="36" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="21">
-        <v>0</v>
-      </c>
-      <c r="C40" s="21">
-        <v>1</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="21">
-        <v>0</v>
-      </c>
-      <c r="B41" s="28">
-        <v>9</v>
-      </c>
-      <c r="C41" s="29">
-        <v>7</v>
-      </c>
-      <c r="D41" s="30">
-        <v>3</v>
-      </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="21">
-        <v>1</v>
-      </c>
-      <c r="B42" s="31">
-        <v>8</v>
-      </c>
-      <c r="C42" s="32">
-        <v>5</v>
-      </c>
-      <c r="D42" s="33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="34">
-        <v>6</v>
-      </c>
-      <c r="C43" s="35">
-        <v>4</v>
-      </c>
-      <c r="D43" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:I5"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B7:D9">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I9">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>